<commit_message>
THE HOTTEST FIX AFTER RELEASE :)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -38,13 +38,13 @@
     <t xml:space="preserve">Декану ФККПІ</t>
   </si>
   <si>
-    <t xml:space="preserve">Азаренко О.В.</t>
+    <t xml:space="preserve">Сидоров</t>
   </si>
   <si>
     <t xml:space="preserve">студентів</t>
   </si>
   <si>
-    <t xml:space="preserve">групи СЗ-221</t>
+    <t xml:space="preserve">групи 117-а</t>
   </si>
   <si>
     <t xml:space="preserve">ЗАЯВА</t>
@@ -52,59 +52,147 @@
   <si>
     <t xml:space="preserve">без порушень встановлених термінів і позитивної підсумкової семестрової модульної рейтингової оцінки,
 просимо Вашого дозволу на звільнення нас від складання семестрового екзамену з даної дисципліни
-провідний викладач ______________________________________ і зарахування відповідної
+провідний викладач Вечерковська А. С. і зарахування відповідної
 підсумкової семестрової рейтингової оцінки.</t>
   </si>
   <si>
-    <t xml:space="preserve">У зв’язку з отриманням у ___-му семестрі 2018/2019 навчального року позитивних підсумкових
-модульних рейтингових оцінок з усіх ____ модулів дисципліни _________________________________
-_______________________________________________________________________________</t>
+    <t xml:space="preserve">У зв’язку з отриманням у 1-му семестрі 2019/2020 навчального року позитивних підсумкових
+модульних рейтингових оцінок з усіх 5 модулів дисципліни
+Основи ООП</t>
   </si>
   <si>
     <t xml:space="preserve">№ п/п</t>
   </si>
   <si>
-    <t xml:space="preserve">Прізвище та ініціали студента</t>
+    <t xml:space="preserve">Прізвище та ініціали
+студента</t>
   </si>
   <si>
     <t xml:space="preserve">Рейтингова оцінка</t>
   </si>
   <si>
-    <t xml:space="preserve">Підпис студента</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Підсумкова модульна (бали)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Підсумкова семестрова модульна рейтингова оцінка</t>
+    <t xml:space="preserve">Підпис
+студента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Підсумкова
+модульна (бали)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Підсумкова
+семестрова
+модульна
+рейтингова оцінка</t>
   </si>
   <si>
     <t xml:space="preserve">Екзаменаційна</t>
   </si>
   <si>
-    <t xml:space="preserve">Підсумкова семестрова рейтингова оцінка</t>
+    <t xml:space="preserve">Підсумкова
+семестрова
+рейтингова оцінка</t>
   </si>
   <si>
     <t xml:space="preserve">
  </t>
   </si>
   <si>
-    <t xml:space="preserve">Мод. №1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мод. №2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мод. №3</t>
+    <t xml:space="preserve">Мод.
+№1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мод.
+№2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мод.
+№3</t>
   </si>
   <si>
     <t xml:space="preserve">Бали</t>
   </si>
   <si>
-    <t xml:space="preserve">Націон. шкала</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Шкала ECTS</t>
+    <t xml:space="preserve">Націон.
+шкала</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шкала
+ECTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Галацюк Т. П.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tn890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5tn8b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kjh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuyf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">978rf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Батрак О. П.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r</t>
   </si>
 </sst>
 </file>
@@ -457,6 +545,110 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <b/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="12"/>
@@ -934,6 +1126,32 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
   </fills>
   <borders>
     <border>
@@ -1763,6 +1981,591 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -2000,193 +2803,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2385,160 +3001,160 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="14" fillId="15" borderId="14" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="15" fillId="16" borderId="15" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="16" fillId="17" borderId="16" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="17" fillId="18" borderId="17" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="18" fillId="19" borderId="18" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="19" fillId="20" borderId="19" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="20" fillId="21" borderId="20" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="21" fillId="22" borderId="21" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="22" fillId="23" borderId="22" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="23" fillId="24" borderId="23" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="24" fillId="25" borderId="24" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="25" fillId="26" borderId="25" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="26" fillId="27" borderId="26" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="27" fillId="28" borderId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="28" fillId="29" borderId="28" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="29" fillId="30" borderId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="30" fillId="31" borderId="30" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="31" fillId="32" borderId="31" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="32" fillId="33" borderId="32" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="33" fillId="34" borderId="33" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="34" fillId="35" borderId="34" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="45" fillId="46" borderId="45" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="46" fillId="47" borderId="46" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="47" fillId="48" borderId="47" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="48" fillId="49" borderId="48" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="49" fillId="50" borderId="49" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="50" fillId="51" borderId="50" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="51" fillId="52" borderId="51" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="52" fillId="53" borderId="52" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="53" fillId="54" borderId="53" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="54" fillId="55" borderId="54" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="55" fillId="56" borderId="55" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="56" fillId="57" borderId="56" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="57" fillId="58" borderId="57" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="58" fillId="59" borderId="58" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="59" fillId="60" borderId="59" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="60" fillId="61" borderId="60" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="61" fillId="62" borderId="61" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="62" fillId="63" borderId="62" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="63" fillId="64" borderId="63" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="64" fillId="65" borderId="64" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf fontId="65" fillId="66" borderId="65" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="66" fillId="67" borderId="66" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2580,43 +3196,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="79" fillId="80" borderId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="80" fillId="81" borderId="80" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="81" fillId="82" borderId="81" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="82" fillId="83" borderId="82" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="83" fillId="84" borderId="83" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="84" fillId="85" borderId="84" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="85" fillId="86" borderId="85" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="86" fillId="87" borderId="86" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="87" fillId="88" borderId="87" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="88" fillId="89" borderId="88" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="89" fillId="90" borderId="89" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="90" fillId="91" borderId="90" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="91" fillId="92" borderId="91" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="92" fillId="93" borderId="92" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2781,7 +3397,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="146" fillId="147" borderId="146" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="147" fillId="148" borderId="147" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2811,6 +3427,84 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="156" fillId="157" borderId="156" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="157" fillId="158" borderId="157" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="158" fillId="159" borderId="158" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="159" fillId="160" borderId="159" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="160" fillId="161" borderId="160" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="161" fillId="162" borderId="161" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="162" fillId="163" borderId="162" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="163" fillId="164" borderId="163" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="164" fillId="165" borderId="164" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="165" fillId="166" borderId="165" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="166" fillId="167" borderId="166" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="167" fillId="168" borderId="167" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="168" fillId="169" borderId="168" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="169" fillId="170" borderId="169" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="170" fillId="171" borderId="170" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="171" fillId="172" borderId="171" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="172" fillId="173" borderId="172" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="173" fillId="174" borderId="173" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="174" fillId="175" borderId="174" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="175" fillId="176" borderId="175" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="176" fillId="177" borderId="176" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="177" fillId="178" borderId="177" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="178" fillId="179" borderId="178" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="179" fillId="180" borderId="179" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="180" fillId="181" borderId="180" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="181" fillId="182" borderId="181" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="182" fillId="183" borderId="182" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3099,19 +3793,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.904761904761905" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="7.357142857142857" customWidth="1"/>
-    <col min="4" max="4" width="8.214285714285714" customWidth="1"/>
-    <col min="5" max="5" width="14.142857142857142" customWidth="1"/>
-    <col min="6" max="6" width="6.571428571428571" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="1" max="1" width="5.523809523809525" customWidth="1"/>
+    <col min="2" max="2" width="18.857142857142858" customWidth="1"/>
+    <col min="3" max="3" width="7.428571428571429" customWidth="1"/>
+    <col min="4" max="4" width="7.571428571428571" customWidth="1"/>
+    <col min="5" max="5" width="9.428571428571429" customWidth="1"/>
+    <col min="6" max="6" width="6.285714285714286" customWidth="1"/>
+    <col min="7" max="7" width="9.714285714285714" customWidth="1"/>
     <col min="8" max="8" width="5.857142857142857" customWidth="1"/>
-    <col min="9" max="9" width="10.285714285714286" customWidth="1"/>
-    <col min="10" max="10" width="8.571428571428571" customWidth="1"/>
-    <col min="11" max="11" width="11.142857142857142" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.142857142857142" customWidth="1"/>
+    <col min="11" max="11" width="9.142857142857142" customWidth="1"/>
     <col min="12" max="12" width="9.428571428571429" customWidth="1"/>
-    <col min="13" max="13" width="9.571428571428571" customWidth="1"/>
+    <col min="13" max="13" width="11.571428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -3237,7 +3931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="28.5" customHeight="1">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" t="s" s="40">
         <v>0</v>
       </c>
@@ -3411,7 +4105,7 @@
       <c r="L9" s="116"/>
       <c r="M9" s="117"/>
     </row>
-    <row r="10" ht="37" customHeight="1">
+    <row r="10" ht="39.5" customHeight="1">
       <c r="A10" t="s" s="118">
         <v>10</v>
       </c>
@@ -3434,7 +4128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" ht="60" customHeight="1">
+    <row r="11" ht="69" customHeight="1">
       <c r="A11" s="119"/>
       <c r="B11" s="122"/>
       <c r="C11" t="s" s="137">
@@ -3493,6 +4187,88 @@
         <v>24</v>
       </c>
       <c r="M12" s="136"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" t="s" s="157">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s" s="158">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s" s="159">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s" s="160">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s" s="161">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s" s="162">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s" s="163">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s" s="164">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s" s="165">
+        <v>33</v>
+      </c>
+      <c r="J13" t="s" s="166">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s" s="167">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s" s="168">
+        <v>36</v>
+      </c>
+      <c r="M13" t="s" s="169">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" t="s" s="170">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s" s="171">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s" s="172">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s" s="173">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s" s="174">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s" s="175">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s" s="176">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s" s="177">
+        <v>44</v>
+      </c>
+      <c r="I14" t="s" s="178">
+        <v>45</v>
+      </c>
+      <c r="J14" t="s" s="179">
+        <v>46</v>
+      </c>
+      <c r="K14" t="s" s="180">
+        <v>47</v>
+      </c>
+      <c r="L14" t="s" s="181">
+        <v>48</v>
+      </c>
+      <c r="M14" t="s" s="182">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>